<commit_message>
Commit small removal changes
</commit_message>
<xml_diff>
--- a/resources/wiring-guide.xlsx
+++ b/resources/wiring-guide.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
   <si>
     <t>Device Type</t>
   </si>
@@ -195,6 +195,24 @@
   </si>
   <si>
     <t>??</t>
+  </si>
+  <si>
+    <t>Encoder</t>
+  </si>
+  <si>
+    <t>Left encoder port A</t>
+  </si>
+  <si>
+    <t>Left encoder port B</t>
+  </si>
+  <si>
+    <t>Right encoder port A</t>
+  </si>
+  <si>
+    <t>Right encoder port B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder </t>
   </si>
 </sst>
 </file>
@@ -521,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,27 +895,27 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -905,7 +923,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -913,14 +931,58 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update variable names to remove redundancy/conflicts
</commit_message>
<xml_diff>
--- a/resources/wiring-guide.xlsx
+++ b/resources/wiring-guide.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RoboRIO" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="152">
   <si>
     <t>Device Type</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>DIO 9</t>
-  </si>
-  <si>
-    <t>leftLineFollower</t>
   </si>
   <si>
     <t>navx</t>
@@ -448,15 +445,6 @@
     <t>DrivetrainSubsystem</t>
   </si>
   <si>
-    <t>midLineFollower</t>
-  </si>
-  <si>
-    <t>rightLinefollower</t>
-  </si>
-  <si>
-    <t>elevatorLimit</t>
-  </si>
-  <si>
     <t>ElevatorSubsystem</t>
   </si>
   <si>
@@ -466,9 +454,6 @@
     <t>CargoSubsystem</t>
   </si>
   <si>
-    <t>HatchSubsystem</t>
-  </si>
-  <si>
     <t>ClimbSubsystem</t>
   </si>
   <si>
@@ -502,31 +487,55 @@
     <t>rightBack</t>
   </si>
   <si>
-    <t>cargoPickup</t>
-  </si>
-  <si>
-    <t>hatchPickup</t>
-  </si>
-  <si>
-    <t>elevatorWinch</t>
-  </si>
-  <si>
-    <t>cargoRotator</t>
-  </si>
-  <si>
-    <t>leftClimb</t>
-  </si>
-  <si>
-    <t>rightClimb</t>
-  </si>
-  <si>
-    <t>hatchPlacer</t>
-  </si>
-  <si>
-    <t>hatchDetachLeft</t>
-  </si>
-  <si>
-    <t>hatchDetachRight</t>
+    <t>HatchPickupSubsystem</t>
+  </si>
+  <si>
+    <t>leftClimbMotor</t>
+  </si>
+  <si>
+    <t>rightClimbMotor</t>
+  </si>
+  <si>
+    <t>HatchPlacerSubsystem</t>
+  </si>
+  <si>
+    <t>pickupSol</t>
+  </si>
+  <si>
+    <t>placerSol</t>
+  </si>
+  <si>
+    <t>detachLeftSol</t>
+  </si>
+  <si>
+    <t>detachRightSol</t>
+  </si>
+  <si>
+    <t>pickupMotor</t>
+  </si>
+  <si>
+    <t>winchMotor</t>
+  </si>
+  <si>
+    <t>rotatorMotor</t>
+  </si>
+  <si>
+    <t>leftSol</t>
+  </si>
+  <si>
+    <t>rightSol</t>
+  </si>
+  <si>
+    <t>leftFollower</t>
+  </si>
+  <si>
+    <t>midFollower</t>
+  </si>
+  <si>
+    <t>rightFollower</t>
+  </si>
+  <si>
+    <t>lowLimitSwitch</t>
   </si>
 </sst>
 </file>
@@ -914,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,19 +939,19 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
@@ -950,147 +959,147 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F5" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F6" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
         <v>78</v>
       </c>
-      <c r="B7" t="s">
-        <v>79</v>
-      </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F7" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" t="s">
         <v>87</v>
       </c>
-      <c r="B8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" t="s">
-        <v>88</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" t="s">
         <v>85</v>
-      </c>
-      <c r="B9" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1104,7 +1113,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,25 +1126,25 @@
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -1147,7 +1156,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -1155,7 +1164,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1164,7 +1173,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <v>12</v>
@@ -1174,18 +1183,18 @@
       </c>
       <c r="G2" s="3"/>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1194,7 +1203,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>13</v>
@@ -1204,18 +1213,18 @@
       </c>
       <c r="G3" s="3"/>
       <c r="H3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -1224,7 +1233,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>14</v>
@@ -1234,18 +1243,18 @@
       </c>
       <c r="G4" s="3"/>
       <c r="H4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1254,7 +1263,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -1264,18 +1273,18 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1284,7 +1293,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1294,18 +1303,18 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -1314,7 +1323,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1324,18 +1333,18 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -1344,7 +1353,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -1356,18 +1365,18 @@
         <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -1376,7 +1385,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -1388,18 +1397,18 @@
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="J9" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -1415,18 +1424,18 @@
       </c>
       <c r="G10" s="3"/>
       <c r="H10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="J10" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -1442,18 +1451,18 @@
       </c>
       <c r="G11" s="3"/>
       <c r="H11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="J11" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -1462,7 +1471,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -1472,18 +1481,18 @@
       </c>
       <c r="G12" s="3"/>
       <c r="H12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="J12" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -1492,7 +1501,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13">
         <v>5</v>
@@ -1502,21 +1511,21 @@
       </c>
       <c r="G13" s="3"/>
       <c r="H13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="J13" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1530,18 +1539,18 @@
       </c>
       <c r="G14" s="3"/>
       <c r="H14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" t="s">
         <v>80</v>
-      </c>
-      <c r="B15" t="s">
-        <v>81</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15">
@@ -1552,53 +1561,53 @@
       </c>
       <c r="G15" s="3"/>
       <c r="H15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="6" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="6">
         <v>1</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1611,14 +1620,14 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1646,13 +1655,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -1660,30 +1669,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1696,8 +1705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,22 +1716,22 @@
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -1731,180 +1740,180 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="G3" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="G4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="G5" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G6" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G7" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="7" t="s">
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update wiring-guide with edited variable names
</commit_message>
<xml_diff>
--- a/resources/wiring-guide.xlsx
+++ b/resources/wiring-guide.xlsx
@@ -415,24 +415,6 @@
     <t>PCM 1</t>
   </si>
   <si>
-    <t>HATCH PICKUP 0--1/6</t>
-  </si>
-  <si>
-    <t>HATCH PLACER 1--1/6</t>
-  </si>
-  <si>
-    <t>HATCH LEFT 1--2/5</t>
-  </si>
-  <si>
-    <t>CLIMB LEFT 0--2/5</t>
-  </si>
-  <si>
-    <t>CLIMB RIGHT 0--2/5</t>
-  </si>
-  <si>
-    <t>HATCH RIGHT 1--3/4</t>
-  </si>
-  <si>
     <t>Java File Location</t>
   </si>
   <si>
@@ -502,15 +484,6 @@
     <t>pickupSol</t>
   </si>
   <si>
-    <t>placerSol</t>
-  </si>
-  <si>
-    <t>detachLeftSol</t>
-  </si>
-  <si>
-    <t>detachRightSol</t>
-  </si>
-  <si>
     <t>pickupMotor</t>
   </si>
   <si>
@@ -536,6 +509,33 @@
   </si>
   <si>
     <t>lowLimitSwitch</t>
+  </si>
+  <si>
+    <t>HATCH PICKUP 1--1/6</t>
+  </si>
+  <si>
+    <t>HATCH PLACER 2--1/6</t>
+  </si>
+  <si>
+    <t>HATCH LEFT 2--2/5</t>
+  </si>
+  <si>
+    <t>HATCH RIGHT 2--3/4</t>
+  </si>
+  <si>
+    <t>CLIMB LEFT 1--2/5</t>
+  </si>
+  <si>
+    <t>CLIMB RIGHT 1--2/5</t>
+  </si>
+  <si>
+    <t>scissorHolder</t>
+  </si>
+  <si>
+    <t>leftLauncher</t>
+  </si>
+  <si>
+    <t>rightLauncher</t>
   </si>
 </sst>
 </file>
@@ -951,7 +951,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
@@ -971,10 +971,10 @@
         <v>90</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -991,10 +991,10 @@
         <v>89</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1011,10 +1011,10 @@
         <v>91</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1031,10 +1031,10 @@
         <v>92</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F5" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1051,10 +1051,10 @@
         <v>93</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F6" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1071,10 +1071,10 @@
         <v>94</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F7" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1088,7 +1088,7 @@
         <v>87</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -1156,7 +1156,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -1186,10 +1186,10 @@
         <v>96</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1216,10 +1216,10 @@
         <v>97</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1246,10 +1246,10 @@
         <v>98</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1276,10 +1276,10 @@
         <v>99</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1306,10 +1306,10 @@
         <v>100</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J6" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1336,15 +1336,15 @@
         <v>101</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J7" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -1368,15 +1368,15 @@
         <v>102</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J8" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -1400,10 +1400,10 @@
         <v>103</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="J9" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1427,10 +1427,10 @@
         <v>104</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="J10" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1454,10 +1454,10 @@
         <v>105</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="J11" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1484,10 +1484,10 @@
         <v>106</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="J12" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1514,10 +1514,10 @@
         <v>107</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="J13" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1542,7 +1542,7 @@
         <v>108</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1564,7 +1564,7 @@
         <v>109</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="6" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1587,7 +1587,7 @@
         <v>110</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1706,7 +1706,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,7 +1740,7 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1751,19 +1751,19 @@
         <v>60</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>61</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1774,19 +1774,19 @@
         <v>60</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>61</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="G3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1797,19 +1797,19 @@
         <v>60</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>62</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="G4" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1820,19 +1820,19 @@
         <v>60</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
         <v>63</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>116</v>
+        <v>146</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="G5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1843,19 +1843,19 @@
         <v>60</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>62</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>114</v>
+        <v>147</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="G6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1866,19 +1866,19 @@
         <v>60</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
         <v>63</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="G7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1889,7 +1889,7 @@
         <v>66</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>64</v>
@@ -1899,7 +1899,7 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1910,7 +1910,7 @@
         <v>67</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
Add coast/brake data to PDP tab of wiring-guide
</commit_message>
<xml_diff>
--- a/resources/wiring-guide.xlsx
+++ b/resources/wiring-guide.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RoboRIO" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="155">
   <si>
     <t>Device Type</t>
   </si>
@@ -536,6 +536,15 @@
   </si>
   <si>
     <t>rightLauncher</t>
+  </si>
+  <si>
+    <t>Brake or Coast?</t>
+  </si>
+  <si>
+    <t>Brake</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
@@ -1110,10 +1119,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,10 +1136,11 @@
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1161,8 +1171,11 @@
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1191,8 +1204,11 @@
       <c r="J2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1221,8 +1237,11 @@
       <c r="J3" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1251,8 +1270,11 @@
       <c r="J4" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1281,8 +1303,11 @@
       <c r="J5" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1311,8 +1336,11 @@
       <c r="J6" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1341,8 +1369,11 @@
       <c r="J7" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>121</v>
       </c>
@@ -1373,8 +1404,11 @@
       <c r="J8" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -1405,8 +1439,11 @@
       <c r="J9" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1432,8 +1469,11 @@
       <c r="J10" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1459,8 +1499,11 @@
       <c r="J11" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1489,8 +1532,11 @@
       <c r="J12" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1519,8 +1565,11 @@
       <c r="J13" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1545,7 +1594,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -1567,7 +1616,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="6" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="6" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>33</v>
       </c>
@@ -1705,7 +1754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update wiring-guide with new variable names
</commit_message>
<xml_diff>
--- a/resources/wiring-guide.xlsx
+++ b/resources/wiring-guide.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="RoboRIO" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="156">
   <si>
     <t>Device Type</t>
   </si>
@@ -484,15 +484,6 @@
     <t>pickupSol</t>
   </si>
   <si>
-    <t>pickupMotor</t>
-  </si>
-  <si>
-    <t>winchMotor</t>
-  </si>
-  <si>
-    <t>rotatorMotor</t>
-  </si>
-  <si>
     <t>leftSol</t>
   </si>
   <si>
@@ -502,15 +493,9 @@
     <t>leftFollower</t>
   </si>
   <si>
-    <t>midFollower</t>
-  </si>
-  <si>
     <t>rightFollower</t>
   </si>
   <si>
-    <t>lowLimitSwitch</t>
-  </si>
-  <si>
     <t>HATCH PICKUP 1--1/6</t>
   </si>
   <si>
@@ -545,6 +530,24 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>winch</t>
+  </si>
+  <si>
+    <t>rotator</t>
+  </si>
+  <si>
+    <t>limitSwitch</t>
+  </si>
+  <si>
+    <t>middleFollower</t>
+  </si>
+  <si>
+    <t>pickup</t>
+  </si>
+  <si>
+    <t>intake</t>
   </si>
 </sst>
 </file>
@@ -932,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1026,7 @@
         <v>116</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1043,7 +1046,7 @@
         <v>116</v>
       </c>
       <c r="F5" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1063,7 +1066,7 @@
         <v>116</v>
       </c>
       <c r="F6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1083,7 +1086,7 @@
         <v>115</v>
       </c>
       <c r="F7" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1121,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,7 +1175,7 @@
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1205,7 +1208,7 @@
         <v>123</v>
       </c>
       <c r="K2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1238,7 +1241,7 @@
         <v>124</v>
       </c>
       <c r="K3" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1271,7 +1274,7 @@
         <v>125</v>
       </c>
       <c r="K4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1304,7 +1307,7 @@
         <v>126</v>
       </c>
       <c r="K5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1337,7 +1340,7 @@
         <v>127</v>
       </c>
       <c r="K6" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1370,7 +1373,7 @@
         <v>128</v>
       </c>
       <c r="K7" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1402,10 +1405,10 @@
         <v>115</v>
       </c>
       <c r="J8" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="K8" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1437,10 +1440,10 @@
         <v>117</v>
       </c>
       <c r="J9" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="K9" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1470,7 +1473,7 @@
         <v>130</v>
       </c>
       <c r="K10" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1500,7 +1503,7 @@
         <v>131</v>
       </c>
       <c r="K11" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1530,10 +1533,10 @@
         <v>117</v>
       </c>
       <c r="J12" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="K12" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1563,10 +1566,10 @@
         <v>129</v>
       </c>
       <c r="J13" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1806,7 +1809,7 @@
         <v>61</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>133</v>
@@ -1829,10 +1832,10 @@
         <v>61</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>149</v>
       </c>
       <c r="G3" t="s">
         <v>132</v>
@@ -1852,10 +1855,10 @@
         <v>62</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>145</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>150</v>
       </c>
       <c r="G4" t="s">
         <v>132</v>
@@ -1875,10 +1878,10 @@
         <v>63</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>151</v>
       </c>
       <c r="G5" t="s">
         <v>132</v>
@@ -1898,10 +1901,10 @@
         <v>62</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G6" t="s">
         <v>118</v>
@@ -1921,10 +1924,10 @@
         <v>63</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G7" t="s">
         <v>118</v>

</xml_diff>

<commit_message>
Update wiring-guide with actual PDP port numbers
</commit_message>
<xml_diff>
--- a/resources/wiring-guide.xlsx
+++ b/resources/wiring-guide.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RoboRIO" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="157">
   <si>
     <t>Device Type</t>
   </si>
@@ -409,9 +409,6 @@
     <t>PCM 2</t>
   </si>
   <si>
-    <t>CAM 6</t>
-  </si>
-  <si>
     <t>PCM 1</t>
   </si>
   <si>
@@ -548,13 +545,19 @@
   </si>
   <si>
     <t>intake</t>
+  </si>
+  <si>
+    <t>Talon SRX (offboard)</t>
+  </si>
+  <si>
+    <t>CAM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -588,6 +591,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -642,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -653,6 +663,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -935,7 +948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -963,7 +976,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
@@ -983,10 +996,10 @@
         <v>90</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1003,10 +1016,10 @@
         <v>89</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1023,10 +1036,10 @@
         <v>91</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1043,10 +1056,10 @@
         <v>92</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1063,10 +1076,10 @@
         <v>93</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1083,10 +1096,10 @@
         <v>94</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1100,7 +1113,7 @@
         <v>87</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -1124,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,13 +1182,13 @@
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1192,7 +1205,7 @@
         <v>17</v>
       </c>
       <c r="E2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2">
         <v>40</v>
@@ -1202,13 +1215,13 @@
         <v>96</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1235,13 +1248,13 @@
         <v>97</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1258,7 +1271,7 @@
         <v>17</v>
       </c>
       <c r="E4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>40</v>
@@ -1268,13 +1281,13 @@
         <v>98</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1301,13 +1314,13 @@
         <v>99</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1334,13 +1347,13 @@
         <v>100</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1367,21 +1380,21 @@
         <v>101</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>155</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1402,21 +1415,21 @@
         <v>102</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>155</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -1437,73 +1450,75 @@
         <v>103</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="10">
         <v>9</v>
       </c>
-      <c r="E10">
-        <v>10</v>
-      </c>
-      <c r="F10">
+      <c r="D10" s="10"/>
+      <c r="E10" s="10">
+        <v>4</v>
+      </c>
+      <c r="F10" s="10">
         <v>30</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" t="s">
+      <c r="G10" s="11"/>
+      <c r="H10" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="I10" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="J10" t="s">
-        <v>130</v>
-      </c>
-      <c r="K10" t="s">
-        <v>149</v>
+      <c r="I10" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="10">
         <v>10</v>
       </c>
-      <c r="E11">
-        <v>11</v>
-      </c>
-      <c r="F11">
+      <c r="D11" s="10"/>
+      <c r="E11" s="10">
+        <v>5</v>
+      </c>
+      <c r="F11" s="10">
         <v>30</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" t="s">
+      <c r="G11" s="11"/>
+      <c r="H11" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="I11" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="J11" t="s">
-        <v>131</v>
-      </c>
-      <c r="K11" t="s">
-        <v>149</v>
+      <c r="I11" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1520,7 +1535,7 @@
         <v>32</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F12">
         <v>30</v>
@@ -1530,13 +1545,13 @@
         <v>106</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1553,7 +1568,7 @@
         <v>32</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F13">
         <v>30</v>
@@ -1563,13 +1578,13 @@
         <v>107</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1594,7 +1609,7 @@
         <v>108</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1606,17 +1621,17 @@
       </c>
       <c r="D15" s="3"/>
       <c r="E15">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F15">
         <v>5</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" t="s">
-        <v>109</v>
+        <v>156</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="6" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1636,10 +1651,10 @@
         <v>37</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1684,6 +1699,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1792,7 +1808,7 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1809,13 +1825,13 @@
         <v>61</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1832,13 +1848,13 @@
         <v>61</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1855,13 +1871,13 @@
         <v>62</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1878,13 +1894,13 @@
         <v>63</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1901,13 +1917,13 @@
         <v>62</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1924,13 +1940,13 @@
         <v>63</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1951,7 +1967,7 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix to-dos and update wiring guide
- Deprecate AutoDrive and PathfinderTest
- Move PID_ID and TIMEOUT_MS to Constants
</commit_message>
<xml_diff>
--- a/resources/wiring-guide.xlsx
+++ b/resources/wiring-guide.xlsx
@@ -403,9 +403,6 @@
     <t>CARGO 1</t>
   </si>
   <si>
-    <t>HATCH_IN 2</t>
-  </si>
-  <si>
     <t>PCM 2</t>
   </si>
   <si>
@@ -551,6 +548,9 @@
   </si>
   <si>
     <t>CAM</t>
+  </si>
+  <si>
+    <t>HATCH 2</t>
   </si>
 </sst>
 </file>
@@ -976,7 +976,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
@@ -996,10 +996,10 @@
         <v>90</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1016,10 +1016,10 @@
         <v>89</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1036,10 +1036,10 @@
         <v>91</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1056,10 +1056,10 @@
         <v>92</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1076,10 +1076,10 @@
         <v>93</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1096,10 +1096,10 @@
         <v>94</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1113,7 +1113,7 @@
         <v>87</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -1138,7 +1138,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,13 +1182,13 @@
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1215,13 +1215,13 @@
         <v>96</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1248,13 +1248,13 @@
         <v>97</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1281,13 +1281,13 @@
         <v>98</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1314,13 +1314,13 @@
         <v>99</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1347,13 +1347,13 @@
         <v>100</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1380,21 +1380,21 @@
         <v>101</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1415,21 +1415,21 @@
         <v>102</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -1450,13 +1450,13 @@
         <v>103</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1481,13 +1481,13 @@
         <v>104</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1512,13 +1512,13 @@
         <v>105</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1545,13 +1545,13 @@
         <v>106</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1575,16 +1575,16 @@
       </c>
       <c r="G13" s="3"/>
       <c r="H13" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1606,10 +1606,10 @@
       </c>
       <c r="G14" s="3"/>
       <c r="H14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1628,10 +1628,10 @@
       </c>
       <c r="G15" s="3"/>
       <c r="H15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="6" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1651,10 +1651,10 @@
         <v>37</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1808,7 +1808,7 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1825,13 +1825,13 @@
         <v>61</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1848,13 +1848,13 @@
         <v>61</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1871,13 +1871,13 @@
         <v>62</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1894,13 +1894,13 @@
         <v>63</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1917,13 +1917,13 @@
         <v>62</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1940,13 +1940,13 @@
         <v>63</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1967,7 +1967,7 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Switch ports in wiring-guide, fix pneumatic direction in HatchPlacer
</commit_message>
<xml_diff>
--- a/resources/wiring-guide.xlsx
+++ b/resources/wiring-guide.xlsx
@@ -1138,7 +1138,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,7 +1271,7 @@
         <v>17</v>
       </c>
       <c r="E4">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>40</v>
@@ -1370,7 +1370,7 @@
         <v>17</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F7">
         <v>40</v>

</xml_diff>

<commit_message>
Edit port numbers on wiring-guide
</commit_message>
<xml_diff>
--- a/resources/wiring-guide.xlsx
+++ b/resources/wiring-guide.xlsx
@@ -56,9 +56,6 @@
     <t>Quadrature</t>
   </si>
   <si>
-    <t>Victor SPX</t>
-  </si>
-  <si>
     <t>DIO 7</t>
   </si>
   <si>
@@ -475,9 +472,6 @@
     <t>HatchPlacerSubsystem</t>
   </si>
   <si>
-    <t>pickupSol</t>
-  </si>
-  <si>
     <t>leftSol</t>
   </si>
   <si>
@@ -541,9 +535,6 @@
     <t>pickup</t>
   </si>
   <si>
-    <t>intake</t>
-  </si>
-  <si>
     <t>Talon SRX (offboard)</t>
   </si>
   <si>
@@ -551,6 +542,28 @@
   </si>
   <si>
     <t>HATCH 2</t>
+  </si>
+  <si>
+    <t>intakeMotor</t>
+  </si>
+  <si>
+    <t>rotatorSol</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Victor SPX </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(needs fix)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -964,19 +977,19 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
@@ -984,147 +997,147 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" t="s">
         <v>77</v>
       </c>
-      <c r="B7" t="s">
-        <v>78</v>
-      </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
         <v>86</v>
       </c>
-      <c r="B8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" t="s">
-        <v>87</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
         <v>84</v>
-      </c>
-      <c r="B9" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1138,7 +1151,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,19 +1171,19 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -1182,18 +1195,18 @@
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1202,7 +1215,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2">
         <v>14</v>
@@ -1212,21 +1225,21 @@
       </c>
       <c r="G2" s="3"/>
       <c r="H2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1235,7 +1248,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <v>13</v>
@@ -1245,21 +1258,21 @@
       </c>
       <c r="G3" s="3"/>
       <c r="H3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -1268,7 +1281,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1278,21 +1291,21 @@
       </c>
       <c r="G4" s="3"/>
       <c r="H4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1301,7 +1314,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -1311,21 +1324,21 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1334,7 +1347,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1344,21 +1357,21 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -1367,7 +1380,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -1377,30 +1390,30 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -1412,30 +1425,30 @@
         <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -1447,21 +1460,21 @@
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>1</v>
@@ -1478,21 +1491,21 @@
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>1</v>
@@ -1509,90 +1522,90 @@
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>156</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F12">
         <v>30</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>156</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F13">
         <v>30</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J13" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1606,18 +1619,18 @@
       </c>
       <c r="G14" s="3"/>
       <c r="H14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s">
         <v>79</v>
-      </c>
-      <c r="B15" t="s">
-        <v>80</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15">
@@ -1628,53 +1641,53 @@
       </c>
       <c r="G15" s="3"/>
       <c r="H15" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="6" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="6">
         <v>1</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1687,14 +1700,14 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1723,13 +1736,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -1737,30 +1750,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1774,7 +1787,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,16 +1803,16 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -1808,180 +1821,180 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="G2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="7" t="s">
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update solenoid ID numbers
</commit_message>
<xml_diff>
--- a/resources/wiring-guide.xlsx
+++ b/resources/wiring-guide.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="154">
   <si>
     <t>Device Type</t>
   </si>
@@ -229,24 +229,6 @@
     <t>PCM number</t>
   </si>
   <si>
-    <t>left climb actuator</t>
-  </si>
-  <si>
-    <t>right climb actuator</t>
-  </si>
-  <si>
-    <t>lower/raise hatch pickup</t>
-  </si>
-  <si>
-    <t>extend/retract hatch placer</t>
-  </si>
-  <si>
-    <t>left hatch placing actuator</t>
-  </si>
-  <si>
-    <t>right hatch placing actuator</t>
-  </si>
-  <si>
     <t>main compressor</t>
   </si>
   <si>
@@ -262,15 +244,6 @@
     <t>double solenoid valve</t>
   </si>
   <si>
-    <t>1,6</t>
-  </si>
-  <si>
-    <t>2,5</t>
-  </si>
-  <si>
-    <t>3,4</t>
-  </si>
-  <si>
     <t>COMPRESSOR OUT</t>
   </si>
   <si>
@@ -310,9 +283,6 @@
     <t>right line follower</t>
   </si>
   <si>
-    <t>lower limit switch on elevator</t>
-  </si>
-  <si>
     <t>Hall effect sensor</t>
   </si>
   <si>
@@ -343,9 +313,6 @@
     <t>MXP</t>
   </si>
   <si>
-    <t>NavX-MXP and 3-D printed cover</t>
-  </si>
-  <si>
     <t>ENC 2, ENC 3</t>
   </si>
   <si>
@@ -424,9 +391,6 @@
     <t>LineFollowerSubsystem</t>
   </si>
   <si>
-    <t>CargoSubsystem</t>
-  </si>
-  <si>
     <t>ClimbSubsystem</t>
   </si>
   <si>
@@ -469,48 +433,12 @@
     <t>rightClimbMotor</t>
   </si>
   <si>
-    <t>HatchPlacerSubsystem</t>
-  </si>
-  <si>
-    <t>leftSol</t>
-  </si>
-  <si>
-    <t>rightSol</t>
-  </si>
-  <si>
     <t>leftFollower</t>
   </si>
   <si>
     <t>rightFollower</t>
   </si>
   <si>
-    <t>HATCH PICKUP 1--1/6</t>
-  </si>
-  <si>
-    <t>HATCH PLACER 2--1/6</t>
-  </si>
-  <si>
-    <t>HATCH LEFT 2--2/5</t>
-  </si>
-  <si>
-    <t>HATCH RIGHT 2--3/4</t>
-  </si>
-  <si>
-    <t>CLIMB LEFT 1--2/5</t>
-  </si>
-  <si>
-    <t>CLIMB RIGHT 1--2/5</t>
-  </si>
-  <si>
-    <t>scissorHolder</t>
-  </si>
-  <si>
-    <t>leftLauncher</t>
-  </si>
-  <si>
-    <t>rightLauncher</t>
-  </si>
-  <si>
     <t>Brake or Coast?</t>
   </si>
   <si>
@@ -523,18 +451,12 @@
     <t>winch</t>
   </si>
   <si>
-    <t>rotator</t>
-  </si>
-  <si>
     <t>limitSwitch</t>
   </si>
   <si>
     <t>middleFollower</t>
   </si>
   <si>
-    <t>pickup</t>
-  </si>
-  <si>
     <t>Talon SRX (offboard)</t>
   </si>
   <si>
@@ -542,12 +464,6 @@
   </si>
   <si>
     <t>HATCH 2</t>
-  </si>
-  <si>
-    <t>intakeMotor</t>
-  </si>
-  <si>
-    <t>rotatorSol</t>
   </si>
   <si>
     <r>
@@ -565,12 +481,87 @@
       <t>(needs fix)</t>
     </r>
   </si>
+  <si>
+    <t>elevator limit switch</t>
+  </si>
+  <si>
+    <t>arm limit switch</t>
+  </si>
+  <si>
+    <t>DIO 5</t>
+  </si>
+  <si>
+    <t>HALL 5</t>
+  </si>
+  <si>
+    <t>ArmSubsystem</t>
+  </si>
+  <si>
+    <t>RSL</t>
+  </si>
+  <si>
+    <t>NavX-MXP and 3-D printed cover (1mm hex screws)</t>
+  </si>
+  <si>
+    <t>armRotator</t>
+  </si>
+  <si>
+    <t>armRotatorClone</t>
+  </si>
+  <si>
+    <t>CargoPickupSubsystem</t>
+  </si>
+  <si>
+    <t>ROT CL 11</t>
+  </si>
+  <si>
+    <t>pickupWheels</t>
+  </si>
+  <si>
+    <t>pickupMotor</t>
+  </si>
+  <si>
+    <t>PCM_2</t>
+  </si>
+  <si>
+    <t>PCM_1</t>
+  </si>
+  <si>
+    <t>cargo pickup rotator clone</t>
+  </si>
+  <si>
+    <t>hatch pickup</t>
+  </si>
+  <si>
+    <t>hatch launchers</t>
+  </si>
+  <si>
+    <t>hatch scissor holders</t>
+  </si>
+  <si>
+    <t>0,7</t>
+  </si>
+  <si>
+    <t>4,3</t>
+  </si>
+  <si>
+    <t>5,2</t>
+  </si>
+  <si>
+    <t>pickupSol</t>
+  </si>
+  <si>
+    <t>scissorSol</t>
+  </si>
+  <si>
+    <t>launcherSol</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,12 +589,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -671,14 +656,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -959,20 +944,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -983,13 +968,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>108</v>
+      <c r="E1" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
@@ -997,147 +982,170 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>111</v>
+        <v>78</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>111</v>
+        <v>77</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>113</v>
+        <v>79</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="F4" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>113</v>
+        <v>80</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="F5" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>113</v>
+        <v>81</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="F6" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>129</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" t="s">
         <v>82</v>
       </c>
-      <c r="D7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>112</v>
+      <c r="E7" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="F7" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
+        <v>131</v>
+      </c>
+      <c r="D8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>135</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1148,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,7 +1172,7 @@
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1177,7 +1185,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>14</v>
@@ -1194,14 +1202,14 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>108</v>
+      <c r="I1" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1225,16 +1233,16 @@
       </c>
       <c r="G2" s="3"/>
       <c r="H2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>111</v>
+        <v>84</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="J2" t="s">
+        <v>108</v>
+      </c>
+      <c r="K2" t="s">
         <v>120</v>
-      </c>
-      <c r="K2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1258,16 +1266,16 @@
       </c>
       <c r="G3" s="3"/>
       <c r="H3" t="s">
-        <v>96</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>111</v>
+        <v>85</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="J3" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="K3" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1291,16 +1299,16 @@
       </c>
       <c r="G4" s="3"/>
       <c r="H4" t="s">
-        <v>97</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>111</v>
+        <v>86</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="J4" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="K4" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1324,16 +1332,16 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" t="s">
-        <v>98</v>
-      </c>
-      <c r="I5" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J5" t="s">
         <v>111</v>
       </c>
-      <c r="J5" t="s">
-        <v>123</v>
-      </c>
       <c r="K5" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1357,16 +1365,16 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" t="s">
-        <v>99</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>111</v>
+        <v>88</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="J6" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="K6" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1390,24 +1398,24 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="I7" s="7" t="s">
-        <v>111</v>
-      </c>
       <c r="J7" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="K7" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1425,24 +1433,24 @@
         <v>8</v>
       </c>
       <c r="H8" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="J8" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="K8" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -1460,253 +1468,291 @@
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>114</v>
+        <v>91</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="J9" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="K9" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="10">
-        <v>9</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10">
-        <v>4</v>
-      </c>
-      <c r="F10" s="10">
+        <v>144</v>
+      </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
         <v>30</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>145</v>
+      <c r="H10" t="s">
+        <v>139</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="J10" t="s">
+        <v>137</v>
+      </c>
+      <c r="K10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="10">
-        <v>10</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10">
-        <v>5</v>
-      </c>
-      <c r="F11" s="10">
+      <c r="C11" s="9">
+        <v>9</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9">
+        <v>4</v>
+      </c>
+      <c r="F11" s="9">
         <v>30</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="I11" s="12" t="s">
+      <c r="G11" s="10"/>
+      <c r="H11" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="J11" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="J11" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="K11" s="10" t="s">
-        <v>145</v>
+      <c r="K11" s="9" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C12">
+        <v>27</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12">
-        <v>11</v>
-      </c>
-      <c r="F12">
+      <c r="C12" s="9">
+        <v>10</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9">
+        <v>5</v>
+      </c>
+      <c r="F12" s="9">
         <v>30</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" t="s">
-        <v>105</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J12" t="s">
-        <v>150</v>
-      </c>
-      <c r="K12" t="s">
-        <v>144</v>
+      <c r="G12" s="10"/>
+      <c r="H12" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
         <v>31</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F13">
         <v>30</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>126</v>
+        <v>94</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="J13" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="K13" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
       <c r="E14">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F14">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" t="s">
-        <v>106</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="J14" t="s">
+        <v>141</v>
+      </c>
+      <c r="K14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>28</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F15">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" t="s">
-        <v>152</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="6" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="J15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" t="s">
+        <v>126</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="5" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C17" s="5">
         <v>1</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="H17" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1742,7 +1788,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -1773,7 +1819,7 @@
         <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1784,10 +1830,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,12 +1842,11 @@
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1812,191 +1857,108 @@
         <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="G2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="G3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" t="s">
         <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="G4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>54</v>
       </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5">
+      <c r="E5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="G6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="G7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="5"/>
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update wiring guide (obsolete now)
</commit_message>
<xml_diff>
--- a/resources/wiring-guide.xlsx
+++ b/resources/wiring-guide.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RoboRIO" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="154">
   <si>
     <t>Device Type</t>
   </si>
@@ -355,9 +355,6 @@
     <t>ELEV 7</t>
   </si>
   <si>
-    <t>ROT 8</t>
-  </si>
-  <si>
     <t>L_CLIMB 9</t>
   </si>
   <si>
@@ -391,9 +388,6 @@
     <t>LineFollowerSubsystem</t>
   </si>
   <si>
-    <t>ClimbSubsystem</t>
-  </si>
-  <si>
     <t>PneumaticSubsystem</t>
   </si>
   <si>
@@ -425,12 +419,6 @@
   </si>
   <si>
     <t>HatchPickupSubsystem</t>
-  </si>
-  <si>
-    <t>leftClimbMotor</t>
-  </si>
-  <si>
-    <t>rightClimbMotor</t>
   </si>
   <si>
     <t>leftFollower</t>
@@ -512,9 +500,6 @@
     <t>CargoPickupSubsystem</t>
   </si>
   <si>
-    <t>ROT CL 11</t>
-  </si>
-  <si>
     <t>pickupWheels</t>
   </si>
   <si>
@@ -555,6 +540,21 @@
   </si>
   <si>
     <t>launcherSol</t>
+  </si>
+  <si>
+    <t>CLIMB 12</t>
+  </si>
+  <si>
+    <t>LED lights</t>
+  </si>
+  <si>
+    <t>unplug</t>
+  </si>
+  <si>
+    <t>ARM 8</t>
+  </si>
+  <si>
+    <t>ARM CL 11</t>
   </si>
 </sst>
 </file>
@@ -947,7 +947,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,7 +974,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
@@ -994,10 +994,10 @@
         <v>78</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1014,10 +1014,10 @@
         <v>77</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1034,10 +1034,10 @@
         <v>79</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1054,10 +1054,10 @@
         <v>80</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1074,15 +1074,15 @@
         <v>81</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s">
         <v>67</v>
@@ -1094,30 +1094,30 @@
         <v>82</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B8" t="s">
         <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1125,13 +1125,13 @@
         <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C9" t="s">
         <v>76</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
@@ -1145,7 +1145,7 @@
         <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1156,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,13 +1203,13 @@
         <v>7</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1236,13 +1236,13 @@
         <v>84</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1269,13 +1269,13 @@
         <v>85</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1302,13 +1302,13 @@
         <v>86</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1335,13 +1335,13 @@
         <v>87</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1368,13 +1368,13 @@
         <v>88</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1401,21 +1401,21 @@
         <v>89</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1436,21 +1436,21 @@
         <v>90</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -1468,24 +1468,24 @@
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>91</v>
+        <v>152</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="J9" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C10">
         <v>11</v>
@@ -1500,16 +1500,16 @@
         <v>30</v>
       </c>
       <c r="H10" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="I10" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J10" t="s">
         <v>133</v>
       </c>
-      <c r="J10" t="s">
-        <v>137</v>
-      </c>
       <c r="K10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1523,24 +1523,20 @@
         <v>9</v>
       </c>
       <c r="D11" s="9"/>
-      <c r="E11" s="9">
-        <v>4</v>
+      <c r="E11" s="9" t="s">
+        <v>151</v>
       </c>
       <c r="F11" s="9">
         <v>30</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>115</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="9"/>
       <c r="K11" s="9" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1554,24 +1550,20 @@
         <v>10</v>
       </c>
       <c r="D12" s="9"/>
-      <c r="E12" s="9">
-        <v>5</v>
+      <c r="E12" s="9" t="s">
+        <v>151</v>
       </c>
       <c r="F12" s="9">
         <v>30</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>116</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="9"/>
       <c r="K12" s="9" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1579,7 +1571,7 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1595,16 +1587,16 @@
       </c>
       <c r="G13" s="3"/>
       <c r="H13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J13" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="K13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1612,7 +1604,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1621,138 +1613,167 @@
         <v>31</v>
       </c>
       <c r="E14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14">
         <v>30</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J14" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="K14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15" s="3"/>
+      <c r="D15" t="s">
+        <v>150</v>
+      </c>
       <c r="E15">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F15">
         <v>20</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" t="s">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <v>30</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>20</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" t="s">
+        <v>122</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="5" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="I15" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="J15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16">
-        <v>7</v>
-      </c>
-      <c r="F16">
-        <v>5</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" t="s">
-        <v>126</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="5" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="5">
-        <v>1</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="5" t="s">
+      <c r="I19" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="G20" s="3"/>
+      <c r="H20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="2" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="2" t="s">
+      <c r="G21" s="3"/>
+      <c r="H21" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1832,7 +1853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1863,12 +1884,12 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
         <v>53</v>
@@ -1877,18 +1898,18 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
         <v>53</v>
@@ -1897,18 +1918,18 @@
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
         <v>53</v>
@@ -1917,13 +1938,13 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1943,7 +1964,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>